<commit_message>
adding new charts to issues
</commit_message>
<xml_diff>
--- a/minix_test_data/github_data/filter_user_dcb314.xlsx
+++ b/minix_test_data/github_data/filter_user_dcb314.xlsx
@@ -361,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1449,6 +1449,22 @@
         <v>62</v>
       </c>
     </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>0</v>
+      </c>
+      <c r="B136">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137">
+        <v>243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>